<commit_message>
Ajeitei os dados de lives
</commit_message>
<xml_diff>
--- a/Dash/grafico_lives_artistas_mais_escutados_data.xlsx
+++ b/Dash/grafico_lives_artistas_mais_escutados_data.xlsx
@@ -40,52 +40,52 @@
     <t xml:space="preserve">Simone e Simaria</t>
   </si>
   <si>
-    <t xml:space="preserve">Luan Santana</t>
-  </si>
-  <si>
     <t xml:space="preserve">Raça Negra</t>
   </si>
   <si>
+    <t xml:space="preserve">Alok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zé Neto e Cristiano</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jorge e Mateus</t>
   </si>
   <si>
-    <t xml:space="preserve">Alok</t>
-  </si>
-  <si>
     <t xml:space="preserve">Péricles</t>
   </si>
   <si>
     <t xml:space="preserve">Sorriso Maroto</t>
   </si>
   <si>
+    <t xml:space="preserve">Thiaguinho</t>
+  </si>
+  <si>
     <t xml:space="preserve">Maiara e Maraisa</t>
   </si>
   <si>
+    <t xml:space="preserve"> Os Barões da Pisadinha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marcos e Belutti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mano Walter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wesley Safadão</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ferrugem</t>
+  </si>
+  <si>
     <t xml:space="preserve">Xand Avião</t>
   </si>
   <si>
-    <t xml:space="preserve">Barões da Pisadinha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pixote</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mano Walter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ferrugem</t>
+    <t xml:space="preserve">Gusttavo Lima</t>
   </si>
   <si>
     <t xml:space="preserve">César Menotti e Fabiano</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bell Marques</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fernando e Sorocaba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leonardo e Zé Felipe</t>
   </si>
 </sst>
 </file>
@@ -95,7 +95,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -116,6 +116,20 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -160,13 +174,25 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -188,11 +214,11 @@
   </sheetPr>
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24:B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.22"/>
   </cols>
@@ -211,7 +237,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>54000000</v>
+        <v>55000000</v>
       </c>
       <c r="C2" s="1"/>
     </row>
@@ -252,7 +278,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>14000000</v>
+        <v>15000000</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -260,7 +286,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>13000000</v>
+        <v>14000000</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -268,7 +294,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>12000000</v>
+        <v>13000000</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -284,15 +310,15 @@
         <v>11</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>9800000</v>
+        <v>10000000</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="0" t="n">
-        <v>7800000</v>
+      <c r="B12" s="2" t="n">
+        <v>10000000</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -300,7 +326,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>7600000</v>
+        <v>9000000</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -308,15 +334,15 @@
         <v>14</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>7500000</v>
+        <v>8300000</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="0" t="n">
-        <v>7100000</v>
+      <c r="B15" s="4" t="n">
+        <v>8000000</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -324,7 +350,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>6700000</v>
+        <v>7800000</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -332,7 +358,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>6000000</v>
+        <v>6700000</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -340,7 +366,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>5800000</v>
+        <v>6700000</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -348,7 +374,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>5300000</v>
+        <v>6200000</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -356,7 +382,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>5200000</v>
+        <v>6200000</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -364,7 +390,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>5200000</v>
+        <v>6000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>